<commit_message>
prueba cerrar sesion, recuperarPW
</commit_message>
<xml_diff>
--- a/Entrega 4/Pruebas/CerrarSesion.xlsx
+++ b/Entrega 4/Pruebas/CerrarSesion.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pepus Perez Flores\Documents\DAW2020\Entrega 4\Pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F089CC50-44F0-4C06-B93A-22BD57DAA355}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC6A0C0-54E4-4D24-A057-EEA5EE0AB552}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>Escenarios alternativos</t>
   </si>
@@ -42,51 +43,9 @@
     <t>Resultado Esperado</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>Salir de interfaz</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
-    <t>A8</t>
-  </si>
-  <si>
-    <t>A9</t>
-  </si>
-  <si>
-    <t>A10</t>
-  </si>
-  <si>
-    <t>A11</t>
-  </si>
-  <si>
     <t>Se perdio la conexión con el servidor</t>
   </si>
   <si>
-    <t>La ventana se cierra sin ningun problema</t>
-  </si>
-  <si>
-    <t>El usuario puede salir en cualquier momento de la pagina</t>
-  </si>
-  <si>
     <t>Despues de cerrar sesion el usuario da click "atrás" del navegador</t>
   </si>
   <si>
@@ -100,13 +59,46 @@
   </si>
   <si>
     <t>Al intentar cerrar la sesion se pierde la conexión al servidor</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Cerrar sesion exitosamente</t>
+  </si>
+  <si>
+    <t>La sesion se cerro exitosamente</t>
+  </si>
+  <si>
+    <t>Se pide volver a hacer login</t>
+  </si>
+  <si>
+    <t>Cerrar pestaña sin cerrar sesion</t>
+  </si>
+  <si>
+    <t>Se cierra la ventana del navegador con la sesion iniciada</t>
+  </si>
+  <si>
+    <t>Browser Abierto</t>
+  </si>
+  <si>
+    <t>Conexión internet activa</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Se cierra la sesion</t>
+  </si>
+  <si>
+    <t>Estado de la prueba</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,13 +124,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -165,10 +169,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -185,8 +190,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -467,14 +489,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.08984375" customWidth="1"/>
     <col min="3" max="3" width="65.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.453125" bestFit="1" customWidth="1"/>
   </cols>
@@ -502,200 +524,192 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="6" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="8" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11"/>
     </row>
     <row r="13" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="11"/>
     </row>
     <row r="14" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="11"/>
     </row>
     <row r="16" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="11"/>
     </row>
     <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="11"/>
     </row>
     <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="6"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="11"/>
     </row>
     <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
     </row>
     <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="6"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="11"/>
     </row>
     <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="6"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="11"/>
     </row>
     <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="6"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="11"/>
     </row>
     <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="6"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="11"/>
     </row>
     <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="6"/>
+      <c r="A25" s="8"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="11"/>
     </row>
     <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="6"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="11"/>
     </row>
     <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="6"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="11"/>
     </row>
     <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="6"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -704,4 +718,405 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BB4C6C8-39B9-40D8-A574-0E6DA2832050}">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="3.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="59.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="20.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="14"/>
+      <c r="B3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="14"/>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="14"/>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="14"/>
+      <c r="B6" s="13">
+        <v>2</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="14"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A8" s="14"/>
+      <c r="B8" s="1">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="14"/>
+      <c r="B9" s="1">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:7" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="14"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A11" s="14"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="14"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="14"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="14"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="14"/>
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A27" s="14"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A28" s="14"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="14"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A30" s="14"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="14"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A33" s="14"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A34" s="14"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="14"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B6:B7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>